<commit_message>
Income and expense details download functionality
</commit_message>
<xml_diff>
--- a/backend/IncomeDetails.xlsx
+++ b/backend/IncomeDetails.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,62 +416,51 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>freelance</v>
+        <v>salary</v>
       </c>
       <c r="B2" t="str">
         <v>30000</v>
       </c>
       <c r="C2" s="1">
-        <v>45987.22928240741</v>
+        <v>45988.22928240741</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>salary</v>
+        <v>Jhjhk</v>
       </c>
       <c r="B3" t="str">
-        <v>80000</v>
+        <v>2222</v>
       </c>
       <c r="C3" s="1">
-        <v>45962.22928240741</v>
+        <v>45983.22928240741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>snacks</v>
+        <v>books</v>
       </c>
       <c r="B4" t="str">
-        <v>500</v>
+        <v>1199</v>
       </c>
       <c r="C4" s="1">
-        <v>45897.22928240741</v>
+        <v>45888.22928240741</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>books</v>
+        <v>groceries</v>
       </c>
       <c r="B5" t="str">
-        <v>1199</v>
+        <v>2200</v>
       </c>
       <c r="C5" s="1">
-        <v>45888.22928240741</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>groceries</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2200</v>
-      </c>
-      <c r="C6" s="1">
         <v>45883.22928240741</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>